<commit_message>
App Data Entry - Contact Details 4 test cases committed
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -137,6 +137,45 @@
   </si>
   <si>
     <t>DS_AT_CD_ADE_CD_09</t>
+  </si>
+  <si>
+    <t>PhoneType</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>ConsentPhoneContact</t>
+  </si>
+  <si>
+    <t>PreferedPhoneContactType</t>
+  </si>
+  <si>
+    <t>EmailType</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>Mobile 1</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Personal Email</t>
+  </si>
+  <si>
+    <t>anglomathews@gmail.com</t>
+  </si>
+  <si>
+    <t>9865745892</t>
+  </si>
+  <si>
+    <t>SpecialChar</t>
+  </si>
+  <si>
+    <t>!@</t>
   </si>
 </sst>
 </file>
@@ -172,7 +211,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,6 +257,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,7 +314,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -287,6 +332,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -636,9 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -715,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -884,20 +937,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:10">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -907,8 +967,29 @@
       <c r="C1" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
@@ -918,8 +999,15 @@
       <c r="C2" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="12"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -929,8 +1017,27 @@
       <c r="C3" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="13"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
@@ -940,8 +1047,15 @@
       <c r="C4" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="12"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
@@ -951,8 +1065,17 @@
       <c r="C5" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="12"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="11" t="s">
         <v>30</v>
       </c>
@@ -962,8 +1085,15 @@
       <c r="C6" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="12"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
@@ -973,8 +1103,15 @@
       <c r="C7" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="12"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="11" t="s">
         <v>34</v>
       </c>
@@ -984,8 +1121,15 @@
       <c r="C8" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="12"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
@@ -995,8 +1139,15 @@
       <c r="C9" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="12"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -1006,8 +1157,19 @@
       <c r="C10" s="12">
         <v>5509</v>
       </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="J5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Consumer durables application details test case commit Stage: Data entry User ID: Anandh
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
-    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId3"/>
+    <sheet name="ApplicationDetails_DataEntry" sheetId="5" r:id="rId3"/>
     <sheet name="ADE_ContactDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -139,49 +140,185 @@
     <t>DS_AT_CD_ADE_CD_09</t>
   </si>
   <si>
-    <t>PhoneType</t>
-  </si>
-  <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
-    <t>ConsentPhoneContact</t>
-  </si>
-  <si>
-    <t>PreferedPhoneContactType</t>
-  </si>
-  <si>
-    <t>EmailType</t>
-  </si>
-  <si>
-    <t>EmailID</t>
-  </si>
-  <si>
-    <t>Mobile 1</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>Personal Email</t>
-  </si>
-  <si>
-    <t>anglomathews@gmail.com</t>
-  </si>
-  <si>
-    <t>9865745892</t>
-  </si>
-  <si>
-    <t>SpecialChar</t>
-  </si>
-  <si>
-    <t>!@</t>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+  </si>
+  <si>
+    <t>product_dropdown</t>
+  </si>
+  <si>
+    <t>sub_product_dropdown</t>
+  </si>
+  <si>
+    <t>total_finance_amount_requested</t>
+  </si>
+  <si>
+    <t>declared_net_income_monthly</t>
+  </si>
+  <si>
+    <t>declared_current_obligation</t>
+  </si>
+  <si>
+    <t>special_promotion_campaign</t>
+  </si>
+  <si>
+    <t>sourcing_channel</t>
+  </si>
+  <si>
+    <t>Business_center_code</t>
+  </si>
+  <si>
+    <t>servicing_type</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>servicing_branch</t>
+  </si>
+  <si>
+    <t>spoke_location</t>
+  </si>
+  <si>
+    <t>closing_staff_servicing_staff_RM</t>
+  </si>
+  <si>
+    <t>topup_type</t>
+  </si>
+  <si>
+    <t>topup_application_number</t>
+  </si>
+  <si>
+    <t>sourcing_type</t>
+  </si>
+  <si>
+    <t>sourcing_office</t>
+  </si>
+  <si>
+    <t>sourcing_entity</t>
+  </si>
+  <si>
+    <t>sourcing_staff</t>
+  </si>
+  <si>
+    <t>reference_type</t>
+  </si>
+  <si>
+    <t>reference_entity</t>
+  </si>
+  <si>
+    <t>reference_code</t>
+  </si>
+  <si>
+    <t>negative_input</t>
+  </si>
+  <si>
+    <t>special_character_input</t>
+  </si>
+  <si>
+    <t>character_input</t>
+  </si>
+  <si>
+    <t>1500000</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>DDA Housing Scheme-2014</t>
+  </si>
+  <si>
+    <t>Digital</t>
+  </si>
+  <si>
+    <t>Business Center-Corporate Banking</t>
+  </si>
+  <si>
+    <t>Financier</t>
+  </si>
+  <si>
+    <t>Saudi National Bank</t>
+  </si>
+  <si>
+    <t>East Zone</t>
+  </si>
+  <si>
+    <t>Akrudi</t>
+  </si>
+  <si>
+    <t>anant</t>
+  </si>
+  <si>
+    <t>BT Topup</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Monic</t>
+  </si>
+  <si>
+    <t>VENDOR</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>-10000</t>
+  </si>
+  <si>
+    <t>!@#$</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>AT_CD_AD_APPDETAILS_01</t>
+  </si>
+  <si>
+    <t>AT_CD_AD_APPDETAILS_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_AD_APPDETAILS_01</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_AD_APPDETAILS_02</t>
+  </si>
+  <si>
+    <t>AT_CD_AD_APPDETAILS_05</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_AD_APPDETAILS_05</t>
+  </si>
+  <si>
+    <t>Consumer Durables</t>
+  </si>
+  <si>
+    <t>CD-</t>
+  </si>
+  <si>
+    <t>L1App Temp</t>
+  </si>
+  <si>
+    <t>userType_076_03</t>
+  </si>
+  <si>
+    <t>0374</t>
+  </si>
+  <si>
+    <t>AT_CD_AD_APPDETAILS_05_PostReq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -211,7 +348,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,7 +399,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -314,7 +463,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -334,23 +483,45 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -689,16 +860,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.49609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -731,7 +904,7 @@
       <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -739,12 +912,27 @@
       </c>
       <c r="D3" s="8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
     <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -758,7 +946,7 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -766,22 +954,475 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.109375" customWidth="1"/>
-    <col min="6" max="6" width="31.109375" customWidth="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="25.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="15" width="35.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="15" width="32.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="15" width="43.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="15" width="32.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="15" width="30.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="15" width="28.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="15" width="32.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="15" width="21.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="15" width="39.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="15" width="15.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="15" width="40.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="15" width="24.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="15" width="31.140625" collapsed="true"/>
+    <col min="15" max="17" customWidth="true" style="15" width="31.28515625" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" style="15" width="15.140625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="15" width="16.7109375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" style="15" width="19.42578125" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="15" width="20.7109375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="15" width="24.0" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="15" width="31.42578125" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="15" width="26.7109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="15" width="19.5703125" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" style="15" width="26.42578125" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" style="15" width="17.5703125" collapsed="true"/>
+    <col min="28" max="16384" style="15" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="16"/>
+      <c r="U3" s="16"/>
+      <c r="V3" s="16"/>
+      <c r="W3" s="16"/>
+      <c r="X3" s="16"/>
+      <c r="Y3" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA3" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="T4" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="W4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="X4" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y4" s="16"/>
+      <c r="Z4" s="16"/>
+      <c r="AA4" s="16"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Z3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="33.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -811,55 +1452,53 @@
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>23</v>
+      <c r="A2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>25</v>
+      <c r="A3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>27</v>
+      <c r="A4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="A5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5"/>
       <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="11" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>8</v>
@@ -867,10 +1506,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>8</v>
@@ -878,10 +1517,10 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>8</v>
@@ -889,10 +1528,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>8</v>
@@ -900,276 +1539,81 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="11" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C10">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="C12:C14">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C14">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1"/>
-    <col min="5" max="5" width="14" style="15" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="23.77734375" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
-    <col min="9" max="9" width="23.88671875" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1"/>
-    <hyperlink ref="J5" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Contact details all testcases committed.......
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
     <sheet name="TestData" sheetId="2" r:id="rId2"/>
     <sheet name="ApplicationDetails_DataEntry" sheetId="5" r:id="rId3"/>
-    <sheet name="ADE_ContactDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="ADE_ContactDetails" sheetId="6" r:id="rId4"/>
     <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="122">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -312,13 +312,84 @@
   </si>
   <si>
     <t>AT_CD_AD_APPDETAILS_05_PostReq</t>
+  </si>
+  <si>
+    <t>PhoneType</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>ConsentPhoneContact</t>
+  </si>
+  <si>
+    <t>PreferedPhoneContactType</t>
+  </si>
+  <si>
+    <t>EmailType</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>SpecialChar</t>
+  </si>
+  <si>
+    <t>InvalidData</t>
+  </si>
+  <si>
+    <t>MatchingData</t>
+  </si>
+  <si>
+    <t>MismatchingData</t>
+  </si>
+  <si>
+    <t>Mobile 1</t>
+  </si>
+  <si>
+    <t>9865745892</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Personal Email</t>
+  </si>
+  <si>
+    <t>anglomathews@gmail.com</t>
+  </si>
+  <si>
+    <t>!@</t>
+  </si>
+  <si>
+    <t>Mobile 2</t>
+  </si>
+  <si>
+    <t>8564127771</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>mathews</t>
+  </si>
+  <si>
+    <t>Elisa</t>
+  </si>
+  <si>
+    <t>kuldheep@yahoo.com</t>
+  </si>
+  <si>
+    <t>CharValues</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -463,7 +534,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -491,37 +562,25 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <condense val="0"/>
@@ -866,12 +925,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.49609375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -946,7 +1005,7 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -960,34 +1019,34 @@
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="15" width="25.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="15" width="35.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="15" width="32.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="15" width="43.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="15" width="32.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="15" width="30.85546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="15" width="28.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="15" width="32.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="15" width="21.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="15" width="39.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="15" width="15.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" style="15" width="40.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="15" width="24.0" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="15" width="31.140625" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" style="15" width="31.28515625" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" style="15" width="15.140625" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" style="15" width="16.7109375" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" style="15" width="19.42578125" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" style="15" width="20.7109375" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" style="15" width="24.0" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" style="15" width="31.42578125" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" style="15" width="26.7109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" style="15" width="19.5703125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" style="15" width="26.42578125" collapsed="true"/>
-    <col min="27" max="27" customWidth="true" style="15" width="17.5703125" collapsed="true"/>
-    <col min="28" max="16384" style="15" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="25.33203125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="24" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="31.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="31.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="24" style="15" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="31.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="26.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="9.109375" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1277,20 +1336,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" style="15" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="12.21875" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:14">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -1300,8 +1370,41 @@
       <c r="C1" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
@@ -1311,8 +1414,19 @@
       <c r="C2" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="12"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="11" t="s">
         <v>24</v>
       </c>
@@ -1322,8 +1436,31 @@
       <c r="C3" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="11" t="s">
         <v>26</v>
       </c>
@@ -1333,8 +1470,19 @@
       <c r="C4" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="12"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="11" t="s">
         <v>28</v>
       </c>
@@ -1344,8 +1492,23 @@
       <c r="C5" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="12"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="11" t="s">
         <v>30</v>
       </c>
@@ -1355,8 +1518,27 @@
       <c r="C6" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
         <v>32</v>
       </c>
@@ -1366,8 +1548,19 @@
       <c r="C7" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="12"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="11" t="s">
         <v>34</v>
       </c>
@@ -1377,8 +1570,19 @@
       <c r="C8" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="12"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
@@ -1388,8 +1592,19 @@
       <c r="C9" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="12"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="11" t="s">
         <v>38</v>
       </c>
@@ -1399,8 +1614,28 @@
       <c r="C10" s="12">
         <v>5509</v>
       </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I3" r:id="rId1"/>
+    <hyperlink ref="J5" r:id="rId2"/>
+    <hyperlink ref="I6" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1409,20 +1644,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="35.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="31.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="40.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="33.7109375" collapsed="true"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1594,18 +1829,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:C14">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Consumer Durable AppData Entry CF Income Details feature commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -12,15 +12,16 @@
     <sheet name="ApplicationDetails_DataEntry" sheetId="5" r:id="rId3"/>
     <sheet name="AppDataEntryEmployementDetails" sheetId="8" r:id="rId4"/>
     <sheet name="ADE_ContactDetails" sheetId="6" r:id="rId5"/>
-    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId6"/>
-    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId7"/>
+    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId6"/>
+    <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId7"/>
+    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="213">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -554,6 +555,111 @@
   </si>
   <si>
     <t>DS_AT_CON_DUR_ADE_AD_03</t>
+  </si>
+  <si>
+    <t>Data Set ID</t>
+  </si>
+  <si>
+    <t>Search Record</t>
+  </si>
+  <si>
+    <t>Lumpsum Amount</t>
+  </si>
+  <si>
+    <t>Pension Amount</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
+    <t>Adjusted %</t>
+  </si>
+  <si>
+    <t>Salary Credited To Bank</t>
+  </si>
+  <si>
+    <t>Bank Name</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Deduction</t>
+  </si>
+  <si>
+    <t>Deduction_Frequency</t>
+  </si>
+  <si>
+    <t>Deduction_Amt</t>
+  </si>
+  <si>
+    <t>Deduction_Adj%</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Mismatched Currency</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_01</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_01_D1</t>
+  </si>
+  <si>
+    <t>CASH RENTAL INCOME</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>HDFC BANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ashok Marg Jaipur Branch </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CASH RENTAL INCOME </t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_02</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_03</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_04</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_05</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_06</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_07</t>
+  </si>
+  <si>
+    <t>AT_CD_APD_CFI_08</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -704,7 +810,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -744,13 +850,110 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -2265,459 +2468,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H29"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C14">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2816,4 +2569,719 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5509</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3393</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1450000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>13000</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="4">
+        <v>85000</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="K2" s="4">
+        <v>100</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1500</v>
+      </c>
+      <c r="R2" s="4">
+        <v>100</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:C11">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C14">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C26">
+    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C26">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:C26">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C37">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C37">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C37">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Committed new feature -- App Data Entry- Customer Reference
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -12,16 +12,17 @@
     <sheet name="ApplicationDetails_DataEntry" sheetId="5" r:id="rId3"/>
     <sheet name="AppDataEntryEmployementDetails" sheetId="8" r:id="rId4"/>
     <sheet name="ADE_ContactDetails" sheetId="6" r:id="rId5"/>
-    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId6"/>
-    <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId7"/>
-    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId8"/>
+    <sheet name="ADE_ReferenceDetails" sheetId="11" r:id="rId6"/>
+    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId7"/>
+    <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId8"/>
+    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="254">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -374,12 +375,6 @@
     <t>Hello</t>
   </si>
   <si>
-    <t>mathews</t>
-  </si>
-  <si>
-    <t>Elisa</t>
-  </si>
-  <si>
     <t>kuldheep@yahoo.com</t>
   </si>
   <si>
@@ -395,9 +390,6 @@
     <t>AT_CD_APD_CFE_01_D1</t>
   </si>
   <si>
-    <t>AT_CD_APD_CFE_02</t>
-  </si>
-  <si>
     <t>AT_CD_APD_CFE_03</t>
   </si>
   <si>
@@ -660,6 +652,138 @@
   </si>
   <si>
     <t>e</t>
+  </si>
+  <si>
+    <t>RelationshipType</t>
+  </si>
+  <si>
+    <t>Salutation</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>IdentificationType</t>
+  </si>
+  <si>
+    <t>IdentificationNbr</t>
+  </si>
+  <si>
+    <t>MobileNumber</t>
+  </si>
+  <si>
+    <t>NoOfYearsKnown</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>RecordID</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_01</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_01</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_02</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_02</t>
+  </si>
+  <si>
+    <t>BROTHER</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>AADHAR</t>
+  </si>
+  <si>
+    <t>985461237720</t>
+  </si>
+  <si>
+    <t>8574961255</t>
+  </si>
+  <si>
+    <t>sample@gmail.com</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_03</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_03</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_04</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_04</t>
+  </si>
+  <si>
+    <t>$#</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_05</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_05</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>8567458822</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_06</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_06</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_07</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_07</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_08</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_08</t>
+  </si>
+  <si>
+    <t>AT_CD_ADE_CR_09</t>
+  </si>
+  <si>
+    <t>DS_AT_CD_ADE_CR_09</t>
+  </si>
+  <si>
+    <t>Mrsss</t>
+  </si>
+  <si>
+    <t>2113</t>
+  </si>
+  <si>
+    <t>Sample email</t>
   </si>
 </sst>
 </file>
@@ -810,7 +934,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -851,157 +975,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1514,12 +1497,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1594,7 +1577,7 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1608,34 +1591,34 @@
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.33203125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.88671875" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="31.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="31.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="31.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="31.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.6640625" style="15" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="26.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="26.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="23" max="23" width="31.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="26.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="9.109375" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1928,25 +1911,25 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1960,45 +1943,45 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="11" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C2" s="4">
         <v>5509</v>
@@ -2017,31 +2000,31 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="11" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C3" s="4">
         <v>5509</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="H3" s="4">
         <v>14378</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J3" s="4">
         <v>75</v>
@@ -2053,16 +2036,16 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="11" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C4" s="4">
         <v>5509</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -2071,20 +2054,20 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="4">
         <v>5509</v>
@@ -2103,10 +2086,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="11" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="4">
         <v>5509</v>
@@ -2121,18 +2104,18 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C7" s="4">
         <v>5509</v>
@@ -2145,12 +2128,12 @@
         <v>6887</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -2164,26 +2147,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14" style="15" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" style="15" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2218,7 +2201,7 @@
         <v>104</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>105</v>
@@ -2328,7 +2311,7 @@
         <v>113</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
@@ -2354,7 +2337,7 @@
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="23" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="21"/>
@@ -2450,10 +2433,10 @@
       <c r="K10" s="21"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>118</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2468,25 +2451,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.77734375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="12" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="14" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:19">
       <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
@@ -2497,234 +2491,439 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>162</v>
+        <v>210</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>163</v>
+        <v>211</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>165</v>
+        <v>213</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>215</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="R1" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="S1" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" s="11" t="s">
-        <v>167</v>
+        <v>220</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>168</v>
+        <v>221</v>
       </c>
       <c r="C2" s="12">
         <v>5509</v>
       </c>
-      <c r="D2" t="s">
-        <v>169</v>
-      </c>
-      <c r="E2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F2" t="s">
-        <v>171</v>
-      </c>
-      <c r="G2">
-        <v>6565</v>
-      </c>
-      <c r="H2" t="s">
-        <v>172</v>
-      </c>
-      <c r="I2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" s="11" t="s">
-        <v>174</v>
+        <v>222</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>175</v>
+        <v>223</v>
       </c>
       <c r="C3" s="12">
         <v>5509</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="D3" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>228</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" s="11" t="s">
-        <v>176</v>
+        <v>233</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>177</v>
+        <v>234</v>
       </c>
       <c r="C4" s="12">
         <v>5509</v>
       </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="H6" s="12"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C8" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C9" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="S10" s="21" t="s">
+        <v>251</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K3" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="25" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>192</v>
-      </c>
-      <c r="R1" s="25" t="s">
-        <v>193</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>194</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+      <c r="D1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
-        <v>196</v>
+        <v>164</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="4">
+        <v>165</v>
+      </c>
+      <c r="C2" s="12">
         <v>5509</v>
       </c>
-      <c r="D2" s="4">
-        <v>3393</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1450000</v>
-      </c>
-      <c r="F2" s="4">
-        <v>13000</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="I2" s="4">
-        <v>85000</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="K2" s="4">
-        <v>100</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>1500</v>
-      </c>
-      <c r="R2" s="4">
-        <v>100</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>204</v>
+      <c r="D2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2">
+        <v>6565</v>
+      </c>
+      <c r="H2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5509</v>
       </c>
     </row>
   </sheetData>
@@ -2734,22 +2933,183 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="4">
+        <v>5509</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3393</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1450000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>13000</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I2" s="4">
+        <v>85000</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" s="4">
+        <v>100</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1500</v>
+      </c>
+      <c r="R2" s="4">
+        <v>100</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2921,10 +3281,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="11" t="s">
-        <v>122</v>
+        <v>220</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>123</v>
+        <v>221</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>8</v>
@@ -2932,10 +3292,10 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="11" t="s">
-        <v>124</v>
+        <v>222</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>123</v>
+        <v>223</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>8</v>
@@ -2943,10 +3303,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="11" t="s">
-        <v>125</v>
+        <v>233</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>123</v>
+        <v>234</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>8</v>
@@ -2954,10 +3314,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="11" t="s">
-        <v>126</v>
+        <v>235</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>123</v>
+        <v>236</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>8</v>
@@ -2965,10 +3325,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="11" t="s">
-        <v>127</v>
+        <v>238</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>123</v>
+        <v>239</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>8</v>
@@ -2976,10 +3336,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="11" t="s">
-        <v>128</v>
+        <v>243</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>123</v>
+        <v>244</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>8</v>
@@ -2987,10 +3347,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="11" t="s">
-        <v>129</v>
+        <v>245</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>123</v>
+        <v>246</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>8</v>
@@ -2998,10 +3358,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="11" t="s">
-        <v>130</v>
+        <v>247</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>131</v>
+        <v>248</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>8</v>
@@ -3009,10 +3369,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="11" t="s">
-        <v>132</v>
+        <v>249</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>133</v>
+        <v>250</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>8</v>
@@ -3020,10 +3380,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="11" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>8</v>
@@ -3031,10 +3391,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="11" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>8</v>
@@ -3042,10 +3402,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="11" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -3053,10 +3413,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="11" t="s">
-        <v>167</v>
+        <v>125</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>8</v>
@@ -3064,10 +3424,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="11" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>8</v>
@@ -3075,10 +3435,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="11" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>177</v>
+        <v>128</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>8</v>
@@ -3086,10 +3446,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="11" t="s">
-        <v>196</v>
+        <v>129</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>197</v>
+        <v>130</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -3097,10 +3457,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="11" t="s">
-        <v>205</v>
+        <v>131</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>8</v>
@@ -3108,10 +3468,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="11" t="s">
-        <v>206</v>
+        <v>133</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>197</v>
+        <v>134</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>8</v>
@@ -3119,10 +3479,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="11" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>197</v>
+        <v>136</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>8</v>
@@ -3130,10 +3490,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="11" t="s">
-        <v>208</v>
+        <v>164</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>8</v>
@@ -3141,10 +3501,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="11" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>8</v>
@@ -3152,10 +3512,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="11" t="s">
-        <v>210</v>
+        <v>173</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>8</v>
@@ -3163,122 +3523,167 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="11" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+  <conditionalFormatting sqref="C2:C33">
+    <cfRule type="cellIs" dxfId="17" priority="29" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C14">
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="25" priority="21" operator="equal">
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15:C26">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+  <conditionalFormatting sqref="C37:C44">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+  <conditionalFormatting sqref="C37:C44">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C37">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C37">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C44">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
consumer durables ADE IdentificationDetails_610 - commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -13,16 +13,17 @@
     <sheet name="AppDataEntryEmployementDetails" sheetId="8" r:id="rId4"/>
     <sheet name="ADE_ContactDetails" sheetId="6" r:id="rId5"/>
     <sheet name="ADE_ReferenceDetails" sheetId="11" r:id="rId6"/>
-    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId7"/>
-    <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId8"/>
-    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId9"/>
+    <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId7"/>
+    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId8"/>
+    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId9"/>
+    <sheet name="ADE_IdentificationDet_610" sheetId="12" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="274">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -784,6 +785,66 @@
   </si>
   <si>
     <t>Sample email</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_01</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_01</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_02</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_02</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_03</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_03</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_04</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_04</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_05</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_05</t>
+  </si>
+  <si>
+    <t>AT_CON_DUR_ADE_ID_06</t>
+  </si>
+  <si>
+    <t>DS_AT_CON_DUR_ADE_ID_06</t>
+  </si>
+  <si>
+    <t>ID TYPE</t>
+  </si>
+  <si>
+    <t>ID TYPE NA</t>
+  </si>
+  <si>
+    <t>ID NUMBER</t>
+  </si>
+  <si>
+    <t>ISSUING AUTHORITY</t>
+  </si>
+  <si>
+    <t>COUNTRY OF ISSUING</t>
+  </si>
+  <si>
+    <t>ID NUMBER CHAR</t>
+  </si>
+  <si>
+    <t>Government of KSA</t>
+  </si>
+  <si>
+    <t>*******</t>
   </si>
 </sst>
 </file>
@@ -984,7 +1045,103 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1497,12 +1654,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1565,6 +1722,197 @@
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2" s="8">
+        <v>89898</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C5" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C6" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1577,7 +1925,7 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1591,34 +1939,34 @@
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.33203125" style="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.88671875" style="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.88671875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.33203125" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.85546875" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="31.109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="31.33203125" style="15" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.6640625" style="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.44140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="31.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="31.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.42578125" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.7109375" style="15" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31.44140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="26.6640625" style="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="26.44140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="9.109375" style="15" collapsed="1"/>
+    <col min="23" max="23" width="31.42578125" style="15" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="26.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.42578125" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="9.140625" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -1914,22 +2262,22 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2147,26 +2495,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.88671875" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2457,27 +2805,27 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.33203125" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.33203125" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="12" style="15" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="14" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.6640625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="14" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.44140625" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -2828,102 +3176,158 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="10" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="E1" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>178</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>185</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="R1" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="T1" s="25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="11" t="s">
-        <v>164</v>
+        <v>193</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="12">
+        <v>194</v>
+      </c>
+      <c r="C2" s="4">
         <v>5509</v>
       </c>
-      <c r="D2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2">
-        <v>6565</v>
-      </c>
-      <c r="H2" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="12">
-        <v>5509</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="12">
-        <v>5509</v>
+      <c r="D2" s="4">
+        <v>3393</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1450000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>13000</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I2" s="4">
+        <v>85000</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K2" s="4">
+        <v>100</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>1500</v>
+      </c>
+      <c r="R2" s="4">
+        <v>100</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2933,760 +3337,798 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T2"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>178</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>179</v>
-      </c>
-      <c r="H1" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>181</v>
-      </c>
-      <c r="J1" s="25" t="s">
-        <v>182</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>183</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>184</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>185</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>186</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>187</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="R1" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="S1" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="11" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B37" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="4">
-        <v>5509</v>
-      </c>
-      <c r="D2" s="4">
-        <v>3393</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1450000</v>
-      </c>
-      <c r="F2" s="4">
-        <v>13000</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="I2" s="4">
-        <v>85000</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="K2" s="4">
-        <v>100</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>1500</v>
-      </c>
-      <c r="R2" s="4">
-        <v>100</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>201</v>
+      <c r="C37" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C33">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C44">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C44">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:C50">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:C50">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.109375" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="11" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B2" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="11" t="s">
+      <c r="C2" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="8">
+        <v>6565</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="11" t="s">
+      <c r="C3" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B4" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C36" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="17" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C44">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C44">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C44">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
App data entry customer details code committed
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="4" activeTab="8"/>
@@ -14,16 +14,17 @@
     <sheet name="ADE_ContactDetails" sheetId="6" r:id="rId5"/>
     <sheet name="ADE_ReferenceDetails" sheetId="11" r:id="rId6"/>
     <sheet name="CDAppDataEntryCFIncomeDetails" sheetId="10" r:id="rId7"/>
-    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId8"/>
-    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId9"/>
-    <sheet name="ADE_IdentificationDet_610" sheetId="12" r:id="rId10"/>
+    <sheet name="DataEntry_CustDetailsTestData" sheetId="13" r:id="rId8"/>
+    <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId9"/>
+    <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId10"/>
+    <sheet name="ADE_IdentificationDet_610" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="370">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -845,6 +846,294 @@
   </si>
   <si>
     <t>*******</t>
+  </si>
+  <si>
+    <t>customer_type</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>id_number</t>
+  </si>
+  <si>
+    <t>search_date_of_birth</t>
+  </si>
+  <si>
+    <t>customer_type_dropdown</t>
+  </si>
+  <si>
+    <t>application_type</t>
+  </si>
+  <si>
+    <t>salutation</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>middle_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>father_first_name</t>
+  </si>
+  <si>
+    <t>father_middle_name</t>
+  </si>
+  <si>
+    <t>father_last_name</t>
+  </si>
+  <si>
+    <t>spouse_first_name</t>
+  </si>
+  <si>
+    <t>spouse_middle_name</t>
+  </si>
+  <si>
+    <t>spouse_last_name</t>
+  </si>
+  <si>
+    <t>no_of_children</t>
+  </si>
+  <si>
+    <t>spouse_status</t>
+  </si>
+  <si>
+    <t>date_of_birth</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>education_level</t>
+  </si>
+  <si>
+    <t>maritail_status</t>
+  </si>
+  <si>
+    <t>nationality</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>residential_status</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>no_of_dependents</t>
+  </si>
+  <si>
+    <t>mothers_maiden_name</t>
+  </si>
+  <si>
+    <t>type_of_residency</t>
+  </si>
+  <si>
+    <t>industry_segmentation</t>
+  </si>
+  <si>
+    <t>is_income_considered</t>
+  </si>
+  <si>
+    <t>customer_profile</t>
+  </si>
+  <si>
+    <t>relationship</t>
+  </si>
+  <si>
+    <t>politically_exposed</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>phone_number</t>
+  </si>
+  <si>
+    <t>mobile_number_primary</t>
+  </si>
+  <si>
+    <t>mobile_number_secondary</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>prefered_contact_method</t>
+  </si>
+  <si>
+    <t>prefered_time_for_contact</t>
+  </si>
+  <si>
+    <t>numeric_input</t>
+  </si>
+  <si>
+    <t>valid_search_input</t>
+  </si>
+  <si>
+    <t>invalid_search_input</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_01</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_DATAENTRY_CUSTDETAILS_01</t>
+  </si>
+  <si>
+    <t>Individual Customer</t>
+  </si>
+  <si>
+    <t>Vikram</t>
+  </si>
+  <si>
+    <t>AADHAR CARD</t>
+  </si>
+  <si>
+    <t>123654789012</t>
+  </si>
+  <si>
+    <t>10-Aug-1998</t>
+  </si>
+  <si>
+    <t>Primary Applicant</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Not Working</t>
+  </si>
+  <si>
+    <t>10-Oct-1998</t>
+  </si>
+  <si>
+    <t>MALE</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>Indian</t>
+  </si>
+  <si>
+    <t>General</t>
+  </si>
+  <si>
+    <t>HINDU</t>
+  </si>
+  <si>
+    <t>Resident</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Shushma</t>
+  </si>
+  <si>
+    <t>Self owned</t>
+  </si>
+  <si>
+    <t>Accomodation</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>Small Software Companies. (Small Software Companies have an employee strength less than 50 people or total turnover less than Rs.50 crore)</t>
+  </si>
+  <si>
+    <t>SON</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Ok</t>
+  </si>
+  <si>
+    <t>9657785656</t>
+  </si>
+  <si>
+    <t>9874556328</t>
+  </si>
+  <si>
+    <t>9654120147</t>
+  </si>
+  <si>
+    <t>test098@gmail.com</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_02</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_DATAENTRY_CUSTDETAILS_02</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_03</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_DATAENTRY_CUSTDETAILS_03</t>
+  </si>
+  <si>
+    <t>Updatedfirstname</t>
+  </si>
+  <si>
+    <t>Updatedmiddlename</t>
+  </si>
+  <si>
+    <t>Updatedlastname</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_04</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_DATAENTRY_CUSTDETAILS_04</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_07</t>
+  </si>
+  <si>
+    <t>DS01_AT_CD_DATAENTRY_CUSTDETAILS_07</t>
+  </si>
+  <si>
+    <t>1245!@#$</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_05</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_06</t>
+  </si>
+  <si>
+    <t>AT_CD_DATAENTRY_CUSTDETAILS_08</t>
+  </si>
+  <si>
+    <t>Test execution status</t>
+  </si>
+  <si>
+    <t>Not executed</t>
   </si>
 </sst>
 </file>
@@ -995,7 +1284,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1039,13 +1328,14 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="52">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1091,6 +1381,306 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1728,6 +2318,123 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" s="8">
+        <v>6565</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5509</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
@@ -1736,15 +2443,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="8" width="20.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3337,798 +4044,1635 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:AX6"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AX16" sqref="AX16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+    <row r="1" spans="1:50">
+      <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="N1" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="Q1" s="13" t="s">
+        <v>288</v>
+      </c>
+      <c r="R1" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="S1" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="T1" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>316</v>
+      </c>
+      <c r="AT1" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="2" spans="1:50">
       <c r="A2" s="16" t="s">
-        <v>86</v>
+        <v>320</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>321</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="AD2" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="AH2" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="AI2" s="17" t="s">
+        <v>342</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="AK2" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="AM2" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="AN2" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="AO2" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="AP2" s="18" t="s">
+        <v>349</v>
+      </c>
+      <c r="AQ2" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="AS2" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+    </row>
+    <row r="3" spans="1:50">
       <c r="A3" s="16" t="s">
-        <v>87</v>
+        <v>353</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>354</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>324</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>325</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU3" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV3" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW3" s="5"/>
+      <c r="AX3" s="5"/>
+    </row>
+    <row r="4" spans="1:50">
       <c r="A4" s="16" t="s">
-        <v>90</v>
+        <v>355</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>356</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>358</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>359</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+      <c r="AU4" s="5"/>
+      <c r="AV4" s="5"/>
+      <c r="AW4" s="5"/>
+      <c r="AX4" s="5"/>
+    </row>
+    <row r="5" spans="1:50">
       <c r="A5" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>223</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>244</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="11" t="s">
-        <v>245</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>246</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B36" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="11" t="s">
-        <v>193</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="11" t="s">
-        <v>206</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>194</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>259</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="11" t="s">
-        <v>260</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>261</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="11" t="s">
-        <v>262</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>8</v>
+        <v>360</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="5"/>
+      <c r="Y5" s="5"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="AU5" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="AV5" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW5" s="5"/>
+      <c r="AX5" s="5"/>
+    </row>
+    <row r="6" spans="1:50">
+      <c r="A6" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="5"/>
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+      <c r="AH6" s="5"/>
+      <c r="AI6" s="5"/>
+      <c r="AJ6" s="5"/>
+      <c r="AK6" s="5"/>
+      <c r="AL6" s="5"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="5"/>
+      <c r="AO6" s="5"/>
+      <c r="AP6" s="5"/>
+      <c r="AQ6" s="5"/>
+      <c r="AR6" s="5"/>
+      <c r="AS6" s="5"/>
+      <c r="AT6" s="5"/>
+      <c r="AU6" s="5"/>
+      <c r="AV6" s="5"/>
+      <c r="AW6" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="AX6" s="19" t="s">
+        <v>364</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="21" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="19" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C44">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C44">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C50">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C50">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C50">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AQ2" r:id="rId1"/>
+    <hyperlink ref="AU3" r:id="rId2"/>
+    <hyperlink ref="AU5" r:id="rId3"/>
+    <hyperlink ref="AX6" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="35.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>146</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="16" t="s">
+        <v>366</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>363</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B42" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="8">
-        <v>6565</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="11" t="s">
+      <c r="C42" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B43" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="11" t="s">
+      <c r="C43" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B44" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="C4" s="12">
-        <v>5509</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="B53" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B54" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="11" t="s">
+        <v>260</v>
+      </c>
+      <c r="B56" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D58">
+    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34">
+    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36">
+    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D44">
+    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:D44">
+    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D50">
+    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D50">
+    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51:D58">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51:D58">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C58">
+      <formula1>"Pass,Fail,Not executed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Address details changes commit (App data entry stage)
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -314,9 +314,6 @@
     <t>userType_076_03</t>
   </si>
   <si>
-    <t>0374</t>
-  </si>
-  <si>
     <t>AT_CD_AD_APPDETAILS_05_PostReq</t>
   </si>
   <si>
@@ -782,9 +779,6 @@
     <t>Mrsss</t>
   </si>
   <si>
-    <t>2113</t>
-  </si>
-  <si>
     <t>Sample email</t>
   </si>
   <si>
@@ -1134,6 +1128,12 @@
   </si>
   <si>
     <t>Not executed</t>
+  </si>
+  <si>
+    <t>0203</t>
+  </si>
+  <si>
+    <t>2115</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1335,7 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="96">
     <dxf>
       <font>
         <condense val="0"/>
@@ -1449,6 +1449,514 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2297,7 +2805,7 @@
         <v>95</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>96</v>
+        <v>368</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>14</v>
@@ -2347,59 +2855,59 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="H1" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="I1" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="C2" s="12">
         <v>5509</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>167</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>168</v>
       </c>
       <c r="G2" s="8">
         <v>6565</v>
       </c>
       <c r="H2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I2" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>171</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>172</v>
       </c>
       <c r="C3" s="12">
         <v>5509</v>
@@ -2413,10 +2921,10 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>173</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="C4" s="12">
         <v>5509</v>
@@ -2465,71 +2973,71 @@
         <v>21</v>
       </c>
       <c r="D1" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>271</v>
-      </c>
       <c r="J1" s="10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C2" s="12">
         <v>5509</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F2" s="8">
         <v>89898</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J2" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>169</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C3" s="12">
         <v>5509</v>
@@ -2545,10 +3053,10 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C4" s="12">
         <v>5509</v>
@@ -2564,10 +3072,10 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C5" s="12">
         <v>5509</v>
@@ -2583,10 +3091,10 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C6" s="12">
         <v>5509</v>
@@ -2602,10 +3110,10 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C7" s="12">
         <v>5509</v>
@@ -2998,45 +3506,45 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>121</v>
       </c>
       <c r="C2" s="4">
         <v>5509</v>
@@ -3055,31 +3563,31 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="C3" s="4">
         <v>5509</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>151</v>
       </c>
       <c r="H3" s="4">
         <v>14378</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J3" s="4">
         <v>75</v>
@@ -3091,16 +3599,16 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="C4" s="4">
         <v>5509</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -3109,20 +3617,20 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="C5" s="4">
         <v>5509</v>
@@ -3141,10 +3649,10 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="C6" s="4">
         <v>5509</v>
@@ -3159,18 +3667,18 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>155</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="C7" s="4">
         <v>5509</v>
@@ -3183,12 +3691,12 @@
         <v>6887</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -3235,37 +3743,37 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="K1" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3301,22 +3809,22 @@
         <v>5509</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E3" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="23" t="s">
         <v>111</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>112</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="24"/>
@@ -3363,10 +3871,10 @@
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="23"/>
@@ -3383,21 +3891,21 @@
         <v>5509</v>
       </c>
       <c r="D6" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="21" t="s">
         <v>114</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>115</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="23" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="21"/>
       <c r="L6" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
@@ -3488,10 +3996,10 @@
       <c r="K10" s="21"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -3546,60 +4054,60 @@
         <v>21</v>
       </c>
       <c r="D1" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="N1" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="M1" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="R1" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="P1" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>220</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>221</v>
       </c>
       <c r="C2" s="12">
         <v>5509</v>
@@ -3623,40 +4131,40 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>222</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>223</v>
       </c>
       <c r="C3" s="12">
         <v>5509</v>
       </c>
       <c r="D3" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>224</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="F3" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="G3" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="22" t="s">
         <v>227</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="I3" s="21" t="s">
         <v>228</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="J3" s="21" t="s">
         <v>229</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="K3" s="24" t="s">
         <v>230</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="L3" s="21" t="s">
         <v>231</v>
-      </c>
-      <c r="L3" s="21" t="s">
-        <v>232</v>
       </c>
       <c r="M3" s="24"/>
       <c r="N3" s="24"/>
@@ -3668,10 +4176,10 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>233</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>234</v>
       </c>
       <c r="C4" s="12">
         <v>5509</v>
@@ -3695,10 +4203,10 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>235</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>236</v>
       </c>
       <c r="C5" s="12">
         <v>5509</v>
@@ -3713,10 +4221,10 @@
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
@@ -3726,10 +4234,10 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>238</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>239</v>
       </c>
       <c r="C6" s="12">
         <v>5509</v>
@@ -3737,10 +4245,10 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>240</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>241</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="21"/>
@@ -3750,10 +4258,10 @@
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P6" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q6" s="21"/>
       <c r="R6" s="21"/>
@@ -3761,10 +4269,10 @@
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>243</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>244</v>
       </c>
       <c r="C7" s="12">
         <v>5509</v>
@@ -3783,17 +4291,17 @@
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="26" t="s">
-        <v>252</v>
+        <v>369</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="C8" s="12">
         <v>5509</v>
@@ -3817,10 +4325,10 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>247</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>248</v>
       </c>
       <c r="C9" s="12">
         <v>5509</v>
@@ -3844,10 +4352,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>249</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>250</v>
       </c>
       <c r="C10" s="12">
         <v>5509</v>
@@ -3867,10 +4375,10 @@
       <c r="P10" s="21"/>
       <c r="Q10" s="21"/>
       <c r="R10" s="21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="S10" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -3918,69 +4426,69 @@
         <v>0</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>175</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>176</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="G1" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="25" t="s">
+      <c r="H1" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="I1" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="J1" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="K1" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="K1" s="25" t="s">
+      <c r="L1" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="L1" s="25" t="s">
+      <c r="M1" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="M1" s="25" t="s">
+      <c r="N1" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="N1" s="25" t="s">
+      <c r="O1" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="P1" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="P1" s="25" t="s">
+      <c r="Q1" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="Q1" s="25" t="s">
+      <c r="R1" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="R1" s="25" t="s">
+      <c r="S1" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="S1" s="25" t="s">
+      <c r="T1" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="T1" s="25" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>193</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>194</v>
       </c>
       <c r="C2" s="4">
         <v>5509</v>
@@ -3995,34 +4503,34 @@
         <v>13000</v>
       </c>
       <c r="G2" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>196</v>
       </c>
       <c r="I2" s="4">
         <v>85000</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K2" s="4">
         <v>100</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M2" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="P2" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q2" s="4">
         <v>1500</v>
@@ -4031,10 +4539,10 @@
         <v>100</v>
       </c>
       <c r="S2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -4111,136 +4619,136 @@
         <v>41</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="F1" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>276</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="M1" s="13" t="s">
         <v>282</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>283</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>287</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>288</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>290</v>
       </c>
-      <c r="T1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>291</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="W1" s="13" t="s">
         <v>292</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="X1" s="13" t="s">
         <v>293</v>
       </c>
-      <c r="W1" s="13" t="s">
+      <c r="Y1" s="13" t="s">
         <v>294</v>
       </c>
-      <c r="X1" s="13" t="s">
+      <c r="Z1" s="13" t="s">
         <v>295</v>
       </c>
-      <c r="Y1" s="13" t="s">
+      <c r="AA1" s="13" t="s">
         <v>296</v>
       </c>
-      <c r="Z1" s="13" t="s">
+      <c r="AB1" s="13" t="s">
         <v>297</v>
       </c>
-      <c r="AA1" s="13" t="s">
+      <c r="AC1" s="13" t="s">
         <v>298</v>
       </c>
-      <c r="AB1" s="13" t="s">
+      <c r="AD1" s="13" t="s">
         <v>299</v>
       </c>
-      <c r="AC1" s="13" t="s">
+      <c r="AE1" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="AD1" s="13" t="s">
+      <c r="AF1" s="13" t="s">
         <v>301</v>
       </c>
-      <c r="AE1" s="13" t="s">
+      <c r="AG1" s="13" t="s">
         <v>302</v>
       </c>
-      <c r="AF1" s="13" t="s">
+      <c r="AH1" s="13" t="s">
         <v>303</v>
       </c>
-      <c r="AG1" s="13" t="s">
+      <c r="AI1" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="AH1" s="13" t="s">
+      <c r="AJ1" s="13" t="s">
         <v>305</v>
       </c>
-      <c r="AI1" s="13" t="s">
+      <c r="AK1" s="13" t="s">
         <v>306</v>
       </c>
-      <c r="AJ1" s="13" t="s">
+      <c r="AL1" s="13" t="s">
         <v>307</v>
       </c>
-      <c r="AK1" s="13" t="s">
+      <c r="AM1" s="13" t="s">
         <v>308</v>
       </c>
-      <c r="AL1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>309</v>
       </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
         <v>310</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AP1" s="13" t="s">
         <v>311</v>
       </c>
-      <c r="AO1" s="13" t="s">
+      <c r="AQ1" s="13" t="s">
         <v>312</v>
       </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
         <v>313</v>
       </c>
-      <c r="AQ1" s="13" t="s">
+      <c r="AS1" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="AR1" s="13" t="s">
+      <c r="AT1" s="13" t="s">
         <v>315</v>
-      </c>
-      <c r="AS1" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="AT1" s="13" t="s">
-        <v>317</v>
       </c>
       <c r="AU1" s="13" t="s">
         <v>65</v>
@@ -4249,147 +4757,147 @@
         <v>66</v>
       </c>
       <c r="AW1" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AX1" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:50">
       <c r="A2" s="16" t="s">
+        <v>318</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>319</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="D2" s="20" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="E2" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="F2" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="H2" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="J2" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="18" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="U2" s="17" t="s">
         <v>327</v>
       </c>
-      <c r="J2" s="17" t="s">
-        <v>225</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="N2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="T2" s="18" t="s">
+      <c r="V2" s="18" t="s">
         <v>328</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="V2" s="18" t="s">
+      <c r="X2" s="17" t="s">
         <v>330</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="Y2" s="17" t="s">
         <v>331</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="Z2" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="AA2" s="17" t="s">
         <v>333</v>
       </c>
-      <c r="Z2" s="17" t="s">
+      <c r="AB2" s="17" t="s">
         <v>334</v>
       </c>
-      <c r="AA2" s="17" t="s">
+      <c r="AC2" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="AB2" s="17" t="s">
+      <c r="AD2" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="AC2" s="17" t="s">
+      <c r="AE2" s="18" t="s">
+        <v>326</v>
+      </c>
+      <c r="AF2" s="18" t="s">
         <v>337</v>
       </c>
-      <c r="AD2" s="17" t="s">
+      <c r="AG2" s="17" t="s">
         <v>338</v>
       </c>
-      <c r="AE2" s="18" t="s">
-        <v>328</v>
-      </c>
-      <c r="AF2" s="18" t="s">
+      <c r="AH2" s="17" t="s">
         <v>339</v>
       </c>
-      <c r="AG2" s="17" t="s">
+      <c r="AI2" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="AH2" s="17" t="s">
+      <c r="AJ2" s="17" t="s">
         <v>341</v>
       </c>
-      <c r="AI2" s="17" t="s">
+      <c r="AK2" s="17" t="s">
         <v>342</v>
       </c>
-      <c r="AJ2" s="17" t="s">
+      <c r="AL2" s="17" t="s">
         <v>343</v>
       </c>
-      <c r="AK2" s="17" t="s">
+      <c r="AM2" s="18" t="s">
         <v>344</v>
       </c>
-      <c r="AL2" s="17" t="s">
+      <c r="AN2" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="AM2" s="18" t="s">
+      <c r="AO2" s="18" t="s">
         <v>346</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AP2" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="AO2" s="18" t="s">
+      <c r="AQ2" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="AP2" s="18" t="s">
+      <c r="AR2" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="AQ2" s="19" t="s">
+      <c r="AS2" s="18" t="s">
         <v>350</v>
-      </c>
-      <c r="AR2" s="17" t="s">
-        <v>351</v>
-      </c>
-      <c r="AS2" s="18" t="s">
-        <v>352</v>
       </c>
       <c r="AT2" s="5"/>
       <c r="AU2" s="5"/>
@@ -4399,25 +4907,25 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="16" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>321</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="G3" s="18" t="s">
         <v>324</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>326</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -4471,10 +4979,10 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" s="16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -4485,13 +4993,13 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="M4" s="18" t="s">
         <v>357</v>
-      </c>
-      <c r="L4" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>359</v>
       </c>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
@@ -4533,10 +5041,10 @@
     </row>
     <row r="5" spans="1:50">
       <c r="A5" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -4595,10 +5103,10 @@
     </row>
     <row r="6" spans="1:50">
       <c r="A6" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -4647,10 +5155,10 @@
       <c r="AU6" s="5"/>
       <c r="AV6" s="5"/>
       <c r="AW6" s="18" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="AX6" s="19" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
@@ -4669,7 +5177,7 @@
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4693,7 +5201,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -4722,7 +5230,7 @@
         <v>88</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>8</v>
@@ -4736,7 +5244,7 @@
         <v>89</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
@@ -4750,7 +5258,7 @@
         <v>91</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>8</v>
@@ -4758,11 +5266,11 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>8</v>
@@ -4770,13 +5278,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="16" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>8</v>
@@ -4784,13 +5292,13 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="16" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>8</v>
@@ -4798,13 +5306,13 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="16" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>8</v>
@@ -4812,13 +5320,13 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="16" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>8</v>
@@ -4826,11 +5334,11 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="16" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
@@ -4838,11 +5346,11 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="16" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -4850,13 +5358,13 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="16" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>8</v>
@@ -4864,11 +5372,11 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="16" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>8</v>
@@ -4882,7 +5390,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>8</v>
@@ -4896,7 +5404,7 @@
         <v>25</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -4910,7 +5418,7 @@
         <v>27</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>8</v>
@@ -4924,7 +5432,7 @@
         <v>29</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
@@ -4938,7 +5446,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>8</v>
@@ -4952,7 +5460,7 @@
         <v>33</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>8</v>
@@ -4966,7 +5474,7 @@
         <v>35</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>8</v>
@@ -4980,7 +5488,7 @@
         <v>37</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>8</v>
@@ -4994,7 +5502,7 @@
         <v>39</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>8</v>
@@ -5002,13 +5510,13 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B23" s="11" t="s">
-        <v>221</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>8</v>
@@ -5016,13 +5524,13 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="B24" s="11" t="s">
-        <v>223</v>
-      </c>
       <c r="C24" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>8</v>
@@ -5030,13 +5538,13 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="B25" s="11" t="s">
-        <v>234</v>
-      </c>
       <c r="C25" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>8</v>
@@ -5044,13 +5552,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B26" s="11" t="s">
         <v>235</v>
       </c>
-      <c r="B26" s="11" t="s">
-        <v>236</v>
-      </c>
       <c r="C26" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>8</v>
@@ -5058,13 +5566,13 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B27" s="11" t="s">
-        <v>239</v>
-      </c>
       <c r="C27" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>8</v>
@@ -5072,13 +5580,13 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="B28" s="11" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>244</v>
-      </c>
       <c r="C28" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>8</v>
@@ -5086,13 +5594,13 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="B29" s="11" t="s">
-        <v>246</v>
-      </c>
       <c r="C29" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>8</v>
@@ -5100,13 +5608,13 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>247</v>
       </c>
-      <c r="B30" s="11" t="s">
-        <v>248</v>
-      </c>
       <c r="C30" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>8</v>
@@ -5114,13 +5622,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="B31" s="11" t="s">
-        <v>250</v>
-      </c>
       <c r="C31" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>8</v>
@@ -5128,13 +5636,13 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>8</v>
@@ -5142,13 +5650,13 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>8</v>
@@ -5156,13 +5664,13 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>8</v>
@@ -5170,13 +5678,13 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>8</v>
@@ -5184,13 +5692,13 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>8</v>
@@ -5198,13 +5706,13 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="11" t="s">
-        <v>128</v>
-      </c>
       <c r="C37" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>8</v>
@@ -5212,13 +5720,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="11" t="s">
-        <v>130</v>
-      </c>
       <c r="C38" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>8</v>
@@ -5226,13 +5734,13 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="11" t="s">
-        <v>132</v>
-      </c>
       <c r="C39" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>8</v>
@@ -5240,13 +5748,13 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B40" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="C40" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>8</v>
@@ -5254,13 +5762,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B41" s="11" t="s">
-        <v>136</v>
-      </c>
       <c r="C41" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>8</v>
@@ -5268,13 +5776,13 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>165</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>8</v>
@@ -5282,13 +5790,13 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>172</v>
-      </c>
       <c r="C43" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>8</v>
@@ -5296,13 +5804,13 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>174</v>
-      </c>
       <c r="C44" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>8</v>
@@ -5310,13 +5818,13 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B45" s="11" t="s">
-        <v>194</v>
-      </c>
       <c r="C45" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D45" s="4" t="s">
         <v>8</v>
@@ -5324,13 +5832,13 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D46" s="4" t="s">
         <v>8</v>
@@ -5338,13 +5846,13 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>8</v>
@@ -5352,13 +5860,13 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>8</v>
@@ -5366,13 +5874,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D49" s="4" t="s">
         <v>8</v>
@@ -5380,13 +5888,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>8</v>
@@ -5394,13 +5902,13 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>8</v>
@@ -5408,13 +5916,13 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>8</v>
@@ -5422,13 +5930,13 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>8</v>
@@ -5436,13 +5944,13 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="11" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>8</v>
@@ -5450,13 +5958,13 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="11" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>8</v>
@@ -5464,13 +5972,13 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="11" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C56" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>8</v>
@@ -5478,13 +5986,13 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>8</v>
@@ -5492,13 +6000,13 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="11" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>8</v>
@@ -5506,132 +6014,234 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D58">
-    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="49" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="67" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="68" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="65" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="66" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="45" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="63" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="64" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="43" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="61" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="59" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="60" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="39" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="57" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="58" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37:D44">
-    <cfRule type="cellIs" dxfId="37" priority="27" operator="equal">
+  <conditionalFormatting sqref="D2:D58">
+    <cfRule type="cellIs" dxfId="81" priority="55" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="56" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37:D44">
-    <cfRule type="cellIs" dxfId="35" priority="25" operator="equal">
+  <conditionalFormatting sqref="D2:D58">
+    <cfRule type="cellIs" dxfId="79" priority="53" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D50">
-    <cfRule type="cellIs" dxfId="33" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="51" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="52" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D50">
-    <cfRule type="cellIs" dxfId="31" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="49" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="50" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="29" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="45" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="46" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="47" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="48" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="25" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="41" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="43" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="44" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="37" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="40" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="61" priority="33" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="34" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="59" priority="35" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="36" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51:D58">
+    <cfRule type="cellIs" dxfId="57" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51:D58">
+    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D58">
+    <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D58">
+    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5649,20 +6259,18 @@
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51:D58">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51:D58">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
-      <formula>"Yes"</formula>
+  <conditionalFormatting sqref="C3:C58">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"Not executed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Document details code commit User ID: Arul
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
+++ b/AzentioAutomationFramework_ConsumerDurables/TestData/ConsumerDurablesTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="12375" windowHeight="10755" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="12372" windowHeight="10752" firstSheet="8" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="LoginCredentials" sheetId="3" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="ConumerDurablesExeSheet" sheetId="1" r:id="rId9"/>
     <sheet name="ADE_AddressDet_610" sheetId="9" r:id="rId10"/>
     <sheet name="ADE_IdentificationDet_610" sheetId="12" r:id="rId11"/>
+    <sheet name="AppDataEntryDocumentDetails" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="424">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -1134,13 +1135,175 @@
   </si>
   <si>
     <t>2115</t>
+  </si>
+  <si>
+    <t>DataSetID</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>DocumentName</t>
+  </si>
+  <si>
+    <t>RequiredAtStage</t>
+  </si>
+  <si>
+    <t>DocumentStatus</t>
+  </si>
+  <si>
+    <t>MandatoryOptional</t>
+  </si>
+  <si>
+    <t>DocumentCategory</t>
+  </si>
+  <si>
+    <t>UploadDate</t>
+  </si>
+  <si>
+    <t>ExpectedReceiptDate</t>
+  </si>
+  <si>
+    <t>DeferralStage</t>
+  </si>
+  <si>
+    <t>DefApprovedBy</t>
+  </si>
+  <si>
+    <t>ChangeInNatureApprovedBy</t>
+  </si>
+  <si>
+    <t>DocumentForm</t>
+  </si>
+  <si>
+    <t>DocumentQuality</t>
+  </si>
+  <si>
+    <t>DocumentReferenceNumber</t>
+  </si>
+  <si>
+    <t>DocumentReceivedBy</t>
+  </si>
+  <si>
+    <t>LocationWhereReceived</t>
+  </si>
+  <si>
+    <t>RackNo</t>
+  </si>
+  <si>
+    <t>ShelfNo</t>
+  </si>
+  <si>
+    <t>BoxNo</t>
+  </si>
+  <si>
+    <t>DateOfExpiry</t>
+  </si>
+  <si>
+    <t>LodgementAmount</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>ValidInput</t>
+  </si>
+  <si>
+    <t>InvalidInput</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_01</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_01_D1</t>
+  </si>
+  <si>
+    <t>Mathews</t>
+  </si>
+  <si>
+    <t>Pan Card</t>
+  </si>
+  <si>
+    <t>L3 Approval</t>
+  </si>
+  <si>
+    <t>Received</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>KYC Document</t>
+  </si>
+  <si>
+    <t>New Application</t>
+  </si>
+  <si>
+    <t>Ketan Jagtap</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Valid and Clear</t>
+  </si>
+  <si>
+    <t>NAGPUR</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_02</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_02_D1</t>
+  </si>
+  <si>
+    <t>#@#@#@</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_03</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_03_D1</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_04</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_04_D1</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_05</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_05_D1</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_06</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_06_D1</t>
+  </si>
+  <si>
+    <t>#####</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_07</t>
+  </si>
+  <si>
+    <t>AT_CR_APD_DC_07_D1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1167,6 +1330,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1284,7 +1455,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
@@ -1329,313 +1500,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="8" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_5f_" xfId="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="70">
     <dxf>
       <font>
         <condense val="0"/>
@@ -2752,12 +2628,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2832,16 +2708,16 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2949,17 +2825,17 @@
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="8" width="20.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="8" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -3128,6 +3004,331 @@
       <c r="K7" s="8"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:AA8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>370</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>371</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>372</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>373</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>374</v>
+      </c>
+      <c r="G1" s="29" t="s">
+        <v>375</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="I1" s="29" t="s">
+        <v>377</v>
+      </c>
+      <c r="J1" s="29" t="s">
+        <v>378</v>
+      </c>
+      <c r="K1" s="29" t="s">
+        <v>379</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>381</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="O1" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="P1" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q1" s="29" t="s">
+        <v>385</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="S1" s="29" t="s">
+        <v>387</v>
+      </c>
+      <c r="T1" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="U1" s="29" t="s">
+        <v>389</v>
+      </c>
+      <c r="V1" s="29" t="s">
+        <v>390</v>
+      </c>
+      <c r="W1" s="29" t="s">
+        <v>391</v>
+      </c>
+      <c r="X1" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E2" t="s">
+        <v>399</v>
+      </c>
+      <c r="F2" t="s">
+        <v>400</v>
+      </c>
+      <c r="G2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H2" t="s">
+        <v>402</v>
+      </c>
+      <c r="K2" t="s">
+        <v>403</v>
+      </c>
+      <c r="L2" t="s">
+        <v>404</v>
+      </c>
+      <c r="M2" t="s">
+        <v>404</v>
+      </c>
+      <c r="N2" t="s">
+        <v>405</v>
+      </c>
+      <c r="O2" t="s">
+        <v>406</v>
+      </c>
+      <c r="P2">
+        <v>895568</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>404</v>
+      </c>
+      <c r="R2" t="s">
+        <v>407</v>
+      </c>
+      <c r="S2">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>5000</v>
+      </c>
+      <c r="X2" t="s">
+        <v>408</v>
+      </c>
+      <c r="Y2">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B3" t="s">
+        <v>410</v>
+      </c>
+      <c r="P3" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y3">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F4" t="s">
+        <v>400</v>
+      </c>
+      <c r="G4" t="s">
+        <v>401</v>
+      </c>
+      <c r="H4" t="s">
+        <v>402</v>
+      </c>
+      <c r="K4" t="s">
+        <v>403</v>
+      </c>
+      <c r="L4" t="s">
+        <v>404</v>
+      </c>
+      <c r="M4" t="s">
+        <v>404</v>
+      </c>
+      <c r="N4" t="s">
+        <v>405</v>
+      </c>
+      <c r="O4" t="s">
+        <v>406</v>
+      </c>
+      <c r="P4">
+        <v>757575</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>404</v>
+      </c>
+      <c r="R4" t="s">
+        <v>407</v>
+      </c>
+      <c r="S4">
+        <v>8</v>
+      </c>
+      <c r="T4">
+        <v>8</v>
+      </c>
+      <c r="U4">
+        <v>8</v>
+      </c>
+      <c r="W4">
+        <v>8000</v>
+      </c>
+      <c r="X4" t="s">
+        <v>414</v>
+      </c>
+      <c r="Y4">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" t="s">
+        <v>416</v>
+      </c>
+      <c r="P5" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="Y5">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" t="s">
+        <v>417</v>
+      </c>
+      <c r="B6" t="s">
+        <v>418</v>
+      </c>
+      <c r="Y6">
+        <v>5509</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
+      <c r="A7" t="s">
+        <v>419</v>
+      </c>
+      <c r="B7" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y7">
+        <v>5509</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>398</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
+      <c r="A8" t="s">
+        <v>422</v>
+      </c>
+      <c r="B8" t="s">
+        <v>423</v>
+      </c>
+      <c r="Y8">
+        <v>5509</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P3" r:id="rId1"/>
+    <hyperlink ref="P5" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3140,7 +3341,7 @@
       <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3154,34 +3355,34 @@
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="35.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="32.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="43.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="30.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="32.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="39.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="40.85546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="25.33203125" style="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="32.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="43.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="32.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="21.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="39.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="40.88671875" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="31.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="31.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.140625" style="15" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="16.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="19.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.7109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="31.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="31.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.109375" style="15" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="16.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="19.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.6640625" style="15" customWidth="1" collapsed="1"/>
     <col min="22" max="22" width="24" style="15" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="31.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="26.7109375" style="15" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="19.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="26.42578125" style="15" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="17.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="28" max="16384" width="9.140625" style="15" collapsed="1"/>
+    <col min="23" max="23" width="31.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="26.6640625" style="15" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="26.44140625" style="15" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="17.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="28" max="16384" width="9.109375" style="15" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -3477,22 +3678,22 @@
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3714,22 +3915,22 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="9" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" style="15" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="23.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12.85546875" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="23.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12.88671875" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.44140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -4020,27 +4221,27 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="18" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.5703125" style="15" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="18.28515625" style="15" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.28515625" style="15" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5546875" style="15" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18.33203125" style="15" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.33203125" style="15" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="12" style="15" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="14" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13.6640625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.6640625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="9.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="18" max="18" width="14" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.44140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4397,28 +4598,28 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="20.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -4558,57 +4759,57 @@
       <selection activeCell="AX16" sqref="AX16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="34.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="15" max="15" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="20.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="8.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="29" max="29" width="17" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="30" max="30" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="18.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="17.6640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="34" max="34" width="22" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="21.109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="8.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="25.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="18.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="44" max="44" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="25.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="47" width="22.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="8.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="23.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="25.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="18.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="24.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="25.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="22.44140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="48" max="48" width="15" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="49" max="49" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="19.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="19.6640625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:50">
@@ -5176,21 +5377,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D58"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="35.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="40.140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="35.109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="40.109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="33.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -6014,262 +6215,262 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D58">
-    <cfRule type="cellIs" dxfId="95" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="93" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="67" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="68" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="91" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="65" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="66" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="89" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="63" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="64" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34">
-    <cfRule type="cellIs" dxfId="87" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="61" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="85" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="59" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="60" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="83" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="57" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="58" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D58">
-    <cfRule type="cellIs" dxfId="81" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="55" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="56" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D58">
-    <cfRule type="cellIs" dxfId="79" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D50">
-    <cfRule type="cellIs" dxfId="77" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D50">
-    <cfRule type="cellIs" dxfId="75" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="73" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="69" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="65" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="37" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="40" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="61" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="33" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D58">
-    <cfRule type="cellIs" dxfId="57" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D58">
-    <cfRule type="cellIs" dxfId="55" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D58">
-    <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D58">
-    <cfRule type="cellIs" dxfId="51" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="49" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="21" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="41" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="17" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="20" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="33" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="16" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="25" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C58">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Not executed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>